<commit_message>
End of day push
Updated Map (navmesh works), created shotgun asset (first pass).
</commit_message>
<xml_diff>
--- a/Documentation_Folder/Asset-List_Daniel.S.xlsx
+++ b/Documentation_Folder/Asset-List_Daniel.S.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s192126\Documents\RepoFolders\Zombie_Proj\Documentation_Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713772C4-DF90-4E6E-A10C-ED24F7B8A531}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF20748B-B67A-40E0-8411-270C92DFA826}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-60" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -152,13 +152,13 @@
     </r>
   </si>
   <si>
-    <t>70cm x 16cm x 22cm</t>
-  </si>
-  <si>
     <t>Poly Count (Half - Tri's)</t>
   </si>
   <si>
     <t>30cm x 30cm x 65cm</t>
+  </si>
+  <si>
+    <t>70cm x 22cm x 16cm</t>
   </si>
 </sst>
 </file>
@@ -641,7 +641,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,7 +661,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -685,7 +685,7 @@
         <v>17</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -703,7 +703,7 @@
         <v>17</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
1st Stage of day
Milestone planner was updated.
2nd pass of shotgun has barrel + receiver welded together. Updated Asset List with new poly count on shotgun.
</commit_message>
<xml_diff>
--- a/Documentation_Folder/Asset-List_Daniel.S.xlsx
+++ b/Documentation_Folder/Asset-List_Daniel.S.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s192126\Documents\RepoFolders\Zombie_Proj\Documentation_Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADBBAEDF-D6A4-4363-9E34-6C9ED24A974E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD75612C-F1F0-438F-9CFB-07B02140E4CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
   <si>
     <t>Purpose</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>1m x 22cm x 16cm</t>
+  </si>
+  <si>
+    <t>300 Polygons</t>
   </si>
 </sst>
 </file>
@@ -641,7 +644,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,7 +683,9 @@
       <c r="C2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="9"/>
+      <c r="D2" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="E2" s="7" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Particle Effect testing added. Metal_Door asset made. Updated documents
Updated Asset List, Milestone Planner, and Art Bible (added phases of feature asset). 2 particle effects were added (fire, and sparkle). Metal door asset modeled, UV's cleaned up, and implemented into game. Make texture for it
</commit_message>
<xml_diff>
--- a/Documentation_Folder/Asset-List_Daniel.S.xlsx
+++ b/Documentation_Folder/Asset-List_Daniel.S.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s192126\Documents\RepoFolders\Zombie_Proj\Documentation_Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FEBF49-F701-4353-8DEA-08FFE4986A91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75855D14-16E5-4166-9867-601643D7F03B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>Purpose</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>Map decoration + barrier</t>
+  </si>
+  <si>
+    <t>64 Polygons</t>
   </si>
 </sst>
 </file>
@@ -729,7 +732,9 @@
       <c r="C4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="10"/>
+      <c r="D4" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="E4" s="8" t="s">
         <v>16</v>
       </c>

</xml_diff>